<commit_message>
Update code: Completed Record Test 00 up to run ID, sequence number not settled.
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Raw Data (2).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Raw Data (2).xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19020" windowHeight="8325"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SG12019401" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -314,13 +314,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="165" formatCode="00000"/>
-    <numFmt numFmtId="166" formatCode="dd\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,27 +340,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -406,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -445,43 +422,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -507,7 +447,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -530,80 +470,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -611,7 +493,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -623,28 +505,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -976,765 +853,949 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S76"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="21"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="4">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="16"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="9"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="12">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="7" t="s">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="8">
+      <c r="D6" s="4">
         <v>100855</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="4">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="4">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="8">
+      <c r="D9" s="4">
         <v>600001</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="4">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="D10" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="4">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="7" t="s">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="4">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="3" t="s">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="12">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="8">
+      <c r="D16" s="4">
         <v>448909</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="7" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="4">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="7" t="s">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="4">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="8">
+      <c r="D18" s="4">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="4">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="8">
+      <c r="D19" s="4">
         <v>65218000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="4">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="8">
+      <c r="D20" s="4">
         <v>65218901</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="8">
+      <c r="D21" s="4">
         <v>81395097</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="12">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="8">
+      <c r="D22" s="4">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="7" t="s">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="4">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="8">
+      <c r="D24" s="4">
         <v>100934</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="4">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="8">
+      <c r="D25" s="4">
         <v>100652</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="7" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="4">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="8">
+      <c r="D26" s="4">
         <v>1001271</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="4">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="8">
+      <c r="D27" s="4">
         <v>1002143</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="7" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="4">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8">
+      <c r="D28" s="4">
         <v>100641</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="12">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="D29" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="4">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="7" t="s">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="4">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="7" t="s">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="4">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="7" t="s">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="4">
+        <v>7</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="12">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="8"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="12">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="7" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="4">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="7" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="4">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="7" t="s">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="4">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="7" t="s">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="4">
+        <v>7</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="8"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="3" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="12">
+        <v>8</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="D40" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="12">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="8">
+      <c r="D41" s="4">
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="12">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="8">
+      <c r="D42" s="4">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-      <c r="B43" s="7" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="4">
+        <v>6</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="29">
+      <c r="D43" s="8">
         <v>1015232301</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="7" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="4">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="4">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="7" t="s">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="4">
+        <v>15</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="8"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="4">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="8"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="7" t="s">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="4">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="8"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="12">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="8">
+      <c r="D49" s="4">
         <v>1680</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="4">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="8">
+      <c r="D50" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="4">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="8"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="7" t="s">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="4">
+        <v>6</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="8"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
-      <c r="B53" s="7" t="s">
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="4">
+        <v>7</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="8"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="12">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="8">
+      <c r="D55" s="4">
         <v>100897</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="3" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="17"/>
+      <c r="B56" s="12">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="8">
+      <c r="D56" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="39"/>
-      <c r="B57" s="3" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17"/>
+      <c r="B57" s="12">
+        <v>6</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="12">
+        <v>4</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="8">
+      <c r="D58" s="4">
         <v>100827</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
-      <c r="B59" s="3" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17"/>
+      <c r="B59" s="12">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="8">
+      <c r="D59" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="39"/>
-      <c r="B60" s="3" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="17"/>
+      <c r="B60" s="12">
+        <v>6</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="D60" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="12">
+        <v>4</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="8">
+      <c r="D61" s="4">
         <v>100699</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="39"/>
-      <c r="B62" s="3" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="17"/>
+      <c r="B62" s="12">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="8">
+      <c r="D62" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="39"/>
-      <c r="B63" s="3" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="17"/>
+      <c r="B63" s="12">
+        <v>6</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="D63" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="12">
+        <v>4</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="8">
+      <c r="D64" s="4">
         <v>101028</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="39"/>
-      <c r="B65" s="3" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="17"/>
+      <c r="B65" s="12">
+        <v>5</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="8">
+      <c r="D65" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="39"/>
-      <c r="B66" s="3" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="17"/>
+      <c r="B66" s="12">
+        <v>6</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="6">
+      <c r="D66" s="3">
         <v>479245</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="12">
+        <v>4</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="8">
+      <c r="D67" s="4">
         <v>1677</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="12">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="8"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="12">
+        <v>2</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="8">
+      <c r="D69" s="4">
         <v>1687</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
-      <c r="B70" s="3" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="12">
         <v>3</v>
       </c>
-      <c r="C70" s="30">
+      <c r="C70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="9">
         <v>360000</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="32" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="12">
+        <v>2</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="8">
+      <c r="D71" s="4">
         <v>1688</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
-      <c r="B72" s="3" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="12">
         <v>3</v>
       </c>
-      <c r="C72" s="30">
+      <c r="C72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="9">
         <v>199.6</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="32" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="12">
+        <v>2</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="8">
+      <c r="D73" s="4">
         <v>1689</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
-      <c r="B74" s="3" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="12">
         <v>3</v>
       </c>
-      <c r="C74" s="31" t="s">
+      <c r="C74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="37" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="12">
+        <v>2</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="8"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="38"/>
-      <c r="B76" s="3" t="s">
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="12">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="8"/>
+      <c r="D76" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A69:A70"/>
     <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A69:A70"/>
     <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A73:A74"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A12:A21"/>
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A64:A66"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>